<commit_message>
Deropapy reading and displaying tabulated coefficient data
</commit_message>
<xml_diff>
--- a/Prototypes/DEROPAPY/DraftCoeff.xlsx
+++ b/Prototypes/DEROPAPY/DraftCoeff.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\ApsimX\Prototypes\DEROPAPY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D69B212F-8866-4334-9161-A08399E20B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3084460-EA49-4F8A-B887-C8860D86411E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D5328FA5-CBDE-423F-97B2-022D8F41F8B7}"/>
+    <workbookView xWindow="-16320" yWindow="-5925" windowWidth="16440" windowHeight="28440" xr2:uid="{D5328FA5-CBDE-423F-97B2-022D8F41F8B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,9 +47,6 @@
     <t>Average temperature for thermal time calculation</t>
   </si>
   <si>
-    <t>(0,  18.0, 26.0, 34.0, 44.0)</t>
-  </si>
-  <si>
     <t>TT_Acc_Y</t>
   </si>
   <si>
@@ -59,9 +56,6 @@
     <t>Thermal time accumulation at average temperature</t>
   </si>
   <si>
-    <t>(0,  10.0, 18.0, 26.0,  0.0)</t>
-  </si>
-  <si>
     <t>StartGrowth_00</t>
   </si>
   <si>
@@ -122,18 +116,12 @@
     <t>Phenology stage code to drive partitioning changes</t>
   </si>
   <si>
-    <t>(0, 1, 2, 3, 4, 5)</t>
-  </si>
-  <si>
     <t>DailyShareToShoot</t>
   </si>
   <si>
     <t>Fractional allocation of total daily biomass assimilation to shoots (without produce)</t>
   </si>
   <si>
-    <t>(0.2, 0.2, 0.2, 0.2, 0.2, 0.2)</t>
-  </si>
-  <si>
     <t>DailyShareFromShootToLeaf</t>
   </si>
   <si>
@@ -161,9 +149,6 @@
     <t>Radiation use efficiency for total plant biomass (global solar radiation)</t>
   </si>
   <si>
-    <t>(1.9, 1.9, 1.9, 1.9, 1.9, 1.9)</t>
-  </si>
-  <si>
     <t>NDemandStages</t>
   </si>
   <si>
@@ -179,9 +164,6 @@
     <t>Maximum percentage of N in shoot biomass</t>
   </si>
   <si>
-    <t>(2, 2, 2, 2, 2, 2)</t>
-  </si>
-  <si>
     <t>Nconc_Min</t>
   </si>
   <si>
@@ -194,18 +176,12 @@
     <t>Supply/Demand for water</t>
   </si>
   <si>
-    <t>(0, 0.5, 0.8,1.0)</t>
-  </si>
-  <si>
     <t>WaterStress_LAI_Y</t>
   </si>
   <si>
     <t>LAI expansion potential for a given water supply/demand</t>
   </si>
   <si>
-    <t>(0, 0.5, 1.0,1.0)</t>
-  </si>
-  <si>
     <t>WaterStress_RUE_X</t>
   </si>
   <si>
@@ -218,9 +194,6 @@
     <t>NitrogenStress_LAI_X</t>
   </si>
   <si>
-    <t>Fraction of N range in plant (e.g., 0.5 is 50% between N min and N max)</t>
-  </si>
-  <si>
     <t>NitrogenStress_LAI_Y</t>
   </si>
   <si>
@@ -251,15 +224,9 @@
     <t>Thermal time accumulation above heat stress critical temperature</t>
   </si>
   <si>
-    <t>(0, 5, 10, 15, 20)</t>
-  </si>
-  <si>
     <t>Share of HI reduction due to heat stress</t>
   </si>
   <si>
-    <t>(0, 0.2, 0.5, 1.0)</t>
-  </si>
-  <si>
     <t>CO2_level_X</t>
   </si>
   <si>
@@ -269,18 +236,12 @@
     <t>Atmospheric CO2 concentration</t>
   </si>
   <si>
-    <t>(0, 280, 350, 550, 1200)</t>
-  </si>
-  <si>
     <t>CO2_RUE_Y</t>
   </si>
   <si>
     <t>Fractional change in RUE for a given CO2 concentration</t>
   </si>
   <si>
-    <t>(0, 0.9, 1, 1.2, 1.5)</t>
-  </si>
-  <si>
     <t>CO2_WaterUse_Y</t>
   </si>
   <si>
@@ -300,6 +261,45 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>(0   18.0  26.0  34.0  44.0)</t>
+  </si>
+  <si>
+    <t>(0   10.0  18.0  26.0   0.0)</t>
+  </si>
+  <si>
+    <t>(0  1  2  3  4  5)</t>
+  </si>
+  <si>
+    <t>(0.2  0.2  0.2  0.2  0.2  0.2)</t>
+  </si>
+  <si>
+    <t>(1.9  1.9  1.9  1.9  1.9  1.9)</t>
+  </si>
+  <si>
+    <t>(2  2  2  2  2  2)</t>
+  </si>
+  <si>
+    <t>(0  0.5  0.8 1.0)</t>
+  </si>
+  <si>
+    <t>(0  0.5  1.0 1.0)</t>
+  </si>
+  <si>
+    <t>Fraction of N range in plant (e.g.  0.5 is 50% between N min and N max)</t>
+  </si>
+  <si>
+    <t>(0  5  10  15  20)</t>
+  </si>
+  <si>
+    <t>(0  0.2  0.5  1.0)</t>
+  </si>
+  <si>
+    <t>(0  280  350  550  1200)</t>
+  </si>
+  <si>
+    <t>(0  0.9  1  1.2  1.5)</t>
   </si>
 </sst>
 </file>
@@ -702,7 +702,7 @@
   <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E34"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -716,19 +716,19 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="B1" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="C1" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
@@ -747,10 +747,10 @@
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>3</v>
+        <v>75</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>3</v>
+        <v>75</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -760,19 +760,19 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>7</v>
+        <v>76</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>7</v>
+        <v>76</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="3"/>
@@ -782,13 +782,13 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="D4" s="2">
         <v>243</v>
@@ -804,13 +804,13 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D5" s="2">
         <v>400</v>
@@ -826,13 +826,13 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D6" s="2">
         <v>736</v>
@@ -848,13 +848,13 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D7" s="2">
         <v>500</v>
@@ -870,13 +870,13 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D8" s="2">
         <v>200</v>
@@ -892,13 +892,13 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="D9" s="2">
         <v>6</v>
@@ -914,13 +914,13 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="D10" s="2">
         <v>0.45</v>
@@ -936,19 +936,19 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="D11" s="2" t="s">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -958,19 +958,19 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
@@ -980,19 +980,19 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -1002,19 +1002,19 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -1024,19 +1024,19 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -1046,19 +1046,19 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="3"/>
@@ -1068,19 +1068,19 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
@@ -1090,19 +1090,19 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="3"/>
@@ -1112,19 +1112,19 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="3"/>
@@ -1134,19 +1134,19 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -1156,19 +1156,19 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>55</v>
+        <v>82</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>55</v>
+        <v>82</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
@@ -1178,19 +1178,19 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -1200,19 +1200,19 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>55</v>
+        <v>82</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>55</v>
+        <v>82</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
@@ -1222,19 +1222,19 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
@@ -1244,19 +1244,19 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>55</v>
+        <v>82</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>55</v>
+        <v>82</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
@@ -1266,19 +1266,19 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
@@ -1288,19 +1288,19 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>55</v>
+        <v>82</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>55</v>
+        <v>82</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
@@ -1310,13 +1310,13 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D28" s="2">
         <v>100</v>
@@ -1332,13 +1332,13 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="D29" s="2">
         <v>30</v>
@@ -1354,19 +1354,19 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
@@ -1376,19 +1376,19 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
@@ -1398,19 +1398,19 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
@@ -1420,19 +1420,19 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
@@ -1442,19 +1442,19 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>

</xml_diff>

<commit_message>
Phenology model and parameter reads from tables working
</commit_message>
<xml_diff>
--- a/Prototypes/DEROPAPY/DraftCoeff.xlsx
+++ b/Prototypes/DEROPAPY/DraftCoeff.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\ApsimX\Prototypes\DEROPAPY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D082DC9A-D759-44B7-B55B-95365529169F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F33511F-05DF-48E6-9F24-4CB6A37AEFF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D5328FA5-CBDE-423F-97B2-022D8F41F8B7}"/>
+    <workbookView xWindow="-16320" yWindow="-5925" windowWidth="16440" windowHeight="28440" xr2:uid="{D5328FA5-CBDE-423F-97B2-022D8F41F8B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="116">
   <si>
     <t>TT_Temp_X</t>
   </si>
@@ -59,9 +59,6 @@
     <t>StartGrowth_00</t>
   </si>
   <si>
-    <t>DOY</t>
-  </si>
-  <si>
     <t>"Earliest" day of year when sowing/end-dorm is resumed every year</t>
   </si>
   <si>
@@ -83,9 +80,6 @@
     <t>Thermal-time accumulation from sowing/end-dorm to START SENESCENCE</t>
   </si>
   <si>
-    <t>Tt_Maturity or Harvest_04</t>
-  </si>
-  <si>
     <t>Thermal-time accumulation from sowing/end-dorm to MATURITY</t>
   </si>
   <si>
@@ -324,6 +318,72 @@
   </si>
   <si>
     <t>Depth that roots achieve when plant is mature</t>
+  </si>
+  <si>
+    <t>Defoliate</t>
+  </si>
+  <si>
+    <t>binary</t>
+  </si>
+  <si>
+    <t>If plant defoliated at the end of the vegetative phase</t>
+  </si>
+  <si>
+    <t>Flowering</t>
+  </si>
+  <si>
+    <t>ReadyToGraze</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>Photoperiod at start and end of response</t>
+  </si>
+  <si>
+    <t>(8.0 16.0)</t>
+  </si>
+  <si>
+    <t>Pp_StartSenescence_03</t>
+  </si>
+  <si>
+    <t>Pp_Maturity_04</t>
+  </si>
+  <si>
+    <t>Tt_Maturity_04</t>
+  </si>
+  <si>
+    <t>(500.0, 600.0)</t>
+  </si>
+  <si>
+    <t>Tt_Dormancy_05</t>
+  </si>
+  <si>
+    <t>Chill_Dormancy_06</t>
+  </si>
+  <si>
+    <t>Tt_Dormancy_06</t>
+  </si>
+  <si>
+    <t>(0.0 30)</t>
+  </si>
+  <si>
+    <t>500 0</t>
+  </si>
+  <si>
+    <t>Chill_Temp_X</t>
+  </si>
+  <si>
+    <t>Chill_Acc_Y</t>
+  </si>
+  <si>
+    <t>(-5.0 0.0 8.0 12.0)</t>
+  </si>
+  <si>
+    <t>(0.0 1.0 1.0 0.0)</t>
+  </si>
+  <si>
+    <t>DAWS</t>
   </si>
 </sst>
 </file>
@@ -723,10 +783,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E99E4926-CB41-4755-AB5E-FEB3656D8BE5}">
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,22 +799,22 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" t="s">
         <v>72</v>
       </c>
-      <c r="B1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C1" t="s">
-        <v>74</v>
-      </c>
       <c r="D1" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -763,16 +823,16 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>90</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>92</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
@@ -790,13 +850,13 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -814,13 +874,13 @@
         <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="2"/>
@@ -832,19 +892,19 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="D5" s="2">
-        <v>243</v>
+        <v>60</v>
       </c>
       <c r="E5" s="2">
-        <v>243</v>
+        <v>60</v>
       </c>
       <c r="F5" s="2">
-        <v>243</v>
+        <v>60</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -853,13 +913,13 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="2">
         <v>400</v>
@@ -877,13 +937,13 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" s="2">
         <v>736</v>
@@ -901,22 +961,22 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>94</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>4</v>
+        <v>95</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="2">
-        <v>500</v>
-      </c>
-      <c r="E8" s="2">
-        <v>500</v>
-      </c>
-      <c r="F8" s="2">
-        <v>500</v>
+        <v>96</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>98</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -925,22 +985,22 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>102</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>4</v>
+        <v>99</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="2">
-        <v>200</v>
-      </c>
-      <c r="E9" s="2">
-        <v>200</v>
-      </c>
-      <c r="F9" s="2">
-        <v>200</v>
+        <v>100</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -949,22 +1009,22 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="2">
-        <v>6</v>
-      </c>
-      <c r="E10" s="2">
-        <v>6</v>
-      </c>
-      <c r="F10" s="2">
-        <v>6</v>
+        <v>13</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -973,22 +1033,22 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>103</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>99</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="2">
-        <v>0.45</v>
-      </c>
-      <c r="E11" s="2">
-        <v>0.45</v>
-      </c>
-      <c r="F11" s="2">
-        <v>0.45</v>
+        <v>100</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -997,22 +1057,22 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>104</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -1021,22 +1081,22 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>26</v>
+        <v>106</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>78</v>
+        <v>14</v>
+      </c>
+      <c r="D13" s="2">
+        <v>200</v>
+      </c>
+      <c r="E13" s="2">
+        <v>200</v>
+      </c>
+      <c r="F13" s="2">
+        <v>200</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -1045,22 +1105,20 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>28</v>
+        <v>111</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>29</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C14" s="1"/>
       <c r="D14" s="2" t="s">
-        <v>78</v>
+        <v>113</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>78</v>
+        <v>113</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>78</v>
+        <v>113</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -1069,22 +1127,20 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>30</v>
+        <v>112</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>31</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C15" s="1"/>
       <c r="D15" s="2" t="s">
-        <v>78</v>
+        <v>114</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>78</v>
+        <v>114</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>78</v>
+        <v>114</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -1093,22 +1149,20 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>32</v>
+        <v>107</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>33</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C16" s="1"/>
       <c r="D16" s="2" t="s">
-        <v>78</v>
+        <v>109</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>78</v>
+        <v>109</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>78</v>
+        <v>109</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
@@ -1117,22 +1171,20 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>34</v>
+        <v>108</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>36</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C17" s="1"/>
       <c r="D17" s="2" t="s">
-        <v>79</v>
+        <v>110</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>79</v>
+        <v>110</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>79</v>
+        <v>110</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
@@ -1141,22 +1193,22 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>77</v>
+        <v>17</v>
+      </c>
+      <c r="D18" s="2">
+        <v>6</v>
+      </c>
+      <c r="E18" s="2">
+        <v>6</v>
+      </c>
+      <c r="F18" s="2">
+        <v>6</v>
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
@@ -1165,22 +1217,22 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>80</v>
+        <v>20</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0.45</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
@@ -1189,22 +1241,22 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
@@ -1213,22 +1265,22 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
@@ -1237,22 +1289,22 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
@@ -1261,22 +1313,22 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
@@ -1285,22 +1337,22 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
@@ -1309,22 +1361,22 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>83</v>
+        <v>34</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
@@ -1333,22 +1385,22 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
@@ -1357,22 +1409,22 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>83</v>
+        <v>39</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
@@ -1381,22 +1433,22 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
@@ -1405,22 +1457,22 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D29" s="2">
-        <v>100</v>
-      </c>
-      <c r="E29" s="2">
-        <v>100</v>
-      </c>
-      <c r="F29" s="2">
-        <v>100</v>
+        <v>43</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
@@ -1429,22 +1481,22 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D30" s="2">
-        <v>30</v>
-      </c>
-      <c r="E30" s="2">
-        <v>30</v>
-      </c>
-      <c r="F30" s="2">
-        <v>30</v>
+        <v>45</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
@@ -1453,22 +1505,22 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
@@ -1477,22 +1529,22 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
@@ -1501,22 +1553,22 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>64</v>
+        <v>19</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
@@ -1525,22 +1577,22 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
@@ -1549,22 +1601,22 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
@@ -1573,22 +1625,22 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>93</v>
+        <v>52</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>94</v>
+        <v>19</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D36" s="2">
-        <v>1500</v>
-      </c>
-      <c r="E36" s="3">
-        <v>3000</v>
-      </c>
-      <c r="F36" s="3">
-        <v>600</v>
+        <v>53</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
@@ -1596,112 +1648,304 @@
       <c r="J36" s="3"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
+      <c r="A37" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D37" s="2">
+        <v>100</v>
+      </c>
+      <c r="E37" s="2">
+        <v>100</v>
+      </c>
+      <c r="F37" s="2">
+        <v>100</v>
+      </c>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
+      <c r="A38" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D38" s="2">
+        <v>30</v>
+      </c>
+      <c r="E38" s="2">
+        <v>30</v>
+      </c>
+      <c r="F38" s="2">
+        <v>30</v>
+      </c>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
+      <c r="A39" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
+      <c r="A40" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>83</v>
+      </c>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
-      <c r="H41" s="4"/>
-      <c r="I41" s="4"/>
-      <c r="J41" s="4"/>
+      <c r="A41" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
+      <c r="A42" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
-      <c r="I43" s="4"/>
-      <c r="J43" s="4"/>
+      <c r="A43" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
-      <c r="H44" s="4"/>
-      <c r="I44" s="4"/>
-      <c r="J44" s="4"/>
+      <c r="A44" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D44" s="2">
+        <v>1500</v>
+      </c>
+      <c r="E44" s="3">
+        <v>3000</v>
+      </c>
+      <c r="F44" s="3">
+        <v>600</v>
+      </c>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
-      <c r="H45" s="4"/>
-      <c r="I45" s="4"/>
-      <c r="J45" s="4"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="4"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="4"/>
+      <c r="J51" s="4"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="4"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>